<commit_message>
Figured out input and diversity vis!
</commit_message>
<xml_diff>
--- a/2018_First_Year_Class.xlsx
+++ b/2018_First_Year_Class.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanner/Desktop/R.projects/ABA_law_admissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30784BF-6C3A-D343-9A3C-F60FF36D0815}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E7F828-57CC-9A4E-A15F-1DD7CE9A1AAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -782,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -796,6 +796,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,12 +1120,12 @@
   <dimension ref="A1:AJ202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
@@ -1145,7 +1152,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>234</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1255,7 +1262,7 @@
       </c>
     </row>
     <row r="2" spans="1:36">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>233</v>
       </c>
       <c r="B2" s="2">
@@ -1365,7 +1372,7 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>192</v>
       </c>
       <c r="B3" s="2">
@@ -1475,7 +1482,7 @@
       </c>
     </row>
     <row r="4" spans="1:36">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="2">
@@ -1585,7 +1592,7 @@
       </c>
     </row>
     <row r="5" spans="1:36">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>163</v>
       </c>
       <c r="B5" s="2">
@@ -1695,7 +1702,7 @@
       </c>
     </row>
     <row r="6" spans="1:36">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>216</v>
       </c>
       <c r="B6" s="2">
@@ -1805,7 +1812,7 @@
       </c>
     </row>
     <row r="7" spans="1:36">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B7" s="2">
@@ -1915,7 +1922,7 @@
       </c>
     </row>
     <row r="8" spans="1:36">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="2">
@@ -2025,7 +2032,7 @@
       </c>
     </row>
     <row r="9" spans="1:36">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B9" s="2">
@@ -2135,7 +2142,7 @@
       </c>
     </row>
     <row r="10" spans="1:36">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>152</v>
       </c>
       <c r="B10" s="2">
@@ -2245,7 +2252,7 @@
       </c>
     </row>
     <row r="11" spans="1:36">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>132</v>
       </c>
       <c r="B11" s="2">
@@ -2355,7 +2362,7 @@
       </c>
     </row>
     <row r="12" spans="1:36">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="2">
@@ -2465,7 +2472,7 @@
       </c>
     </row>
     <row r="13" spans="1:36">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>84</v>
       </c>
       <c r="B13" s="2">
@@ -2575,7 +2582,7 @@
       </c>
     </row>
     <row r="14" spans="1:36">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>199</v>
       </c>
       <c r="B14" s="2">
@@ -2685,7 +2692,7 @@
       </c>
     </row>
     <row r="15" spans="1:36">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="2">
@@ -2795,7 +2802,7 @@
       </c>
     </row>
     <row r="16" spans="1:36">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B16" s="2">
@@ -2905,7 +2912,7 @@
       </c>
     </row>
     <row r="17" spans="1:36">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B17" s="2">
@@ -3015,7 +3022,7 @@
       </c>
     </row>
     <row r="18" spans="1:36">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>145</v>
       </c>
       <c r="B18" s="2">
@@ -3125,7 +3132,7 @@
       </c>
     </row>
     <row r="19" spans="1:36">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>213</v>
       </c>
       <c r="B19" s="2">
@@ -3235,7 +3242,7 @@
       </c>
     </row>
     <row r="20" spans="1:36">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>57</v>
       </c>
       <c r="B20" s="2">
@@ -3345,7 +3352,7 @@
       </c>
     </row>
     <row r="21" spans="1:36">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>153</v>
       </c>
       <c r="B21" s="2">
@@ -3455,7 +3462,7 @@
       </c>
     </row>
     <row r="22" spans="1:36">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="2"/>
@@ -3563,7 +3570,7 @@
       </c>
     </row>
     <row r="23" spans="1:36">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
         <v>94</v>
       </c>
       <c r="B23" s="2"/>
@@ -3671,7 +3678,7 @@
       </c>
     </row>
     <row r="24" spans="1:36">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="2">
@@ -3781,7 +3788,7 @@
       </c>
     </row>
     <row r="25" spans="1:36">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B25" s="2">
@@ -3891,7 +3898,7 @@
       </c>
     </row>
     <row r="26" spans="1:36">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="6" t="s">
         <v>221</v>
       </c>
       <c r="B26" s="2">
@@ -4001,7 +4008,7 @@
       </c>
     </row>
     <row r="27" spans="1:36">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B27" s="2"/>
@@ -4109,7 +4116,7 @@
       </c>
     </row>
     <row r="28" spans="1:36">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="6" t="s">
         <v>93</v>
       </c>
       <c r="B28" s="2"/>
@@ -4217,7 +4224,7 @@
       </c>
     </row>
     <row r="29" spans="1:36">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="6" t="s">
         <v>219</v>
       </c>
       <c r="B29" s="2"/>
@@ -4325,7 +4332,7 @@
       </c>
     </row>
     <row r="30" spans="1:36">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="2"/>
@@ -4433,7 +4440,7 @@
       </c>
     </row>
     <row r="31" spans="1:36">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B31" s="2"/>
@@ -4541,7 +4548,7 @@
       </c>
     </row>
     <row r="32" spans="1:36">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="6" t="s">
         <v>215</v>
       </c>
       <c r="B32" s="2"/>
@@ -4649,7 +4656,7 @@
       </c>
     </row>
     <row r="33" spans="1:36">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B33" s="2">
@@ -4759,7 +4766,7 @@
       </c>
     </row>
     <row r="34" spans="1:36">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="6" t="s">
         <v>220</v>
       </c>
       <c r="B34">
@@ -4869,7 +4876,7 @@
       </c>
     </row>
     <row r="35" spans="1:36">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="6" t="s">
         <v>98</v>
       </c>
       <c r="B35" s="2"/>
@@ -4977,7 +4984,7 @@
       </c>
     </row>
     <row r="36" spans="1:36">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="6" t="s">
         <v>198</v>
       </c>
       <c r="B36" s="2"/>
@@ -5085,7 +5092,7 @@
       </c>
     </row>
     <row r="37" spans="1:36">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="6" t="s">
         <v>210</v>
       </c>
       <c r="B37" s="2"/>
@@ -5193,7 +5200,7 @@
       </c>
     </row>
     <row r="38" spans="1:36">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="2">
@@ -5303,7 +5310,7 @@
       </c>
     </row>
     <row r="39" spans="1:36">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="6" t="s">
         <v>170</v>
       </c>
       <c r="B39" s="2"/>
@@ -5411,7 +5418,7 @@
       </c>
     </row>
     <row r="40" spans="1:36">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="6" t="s">
         <v>108</v>
       </c>
       <c r="B40" s="2"/>
@@ -5519,7 +5526,7 @@
       </c>
     </row>
     <row r="41" spans="1:36">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B41" s="2"/>
@@ -5627,7 +5634,7 @@
       </c>
     </row>
     <row r="42" spans="1:36">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="6" t="s">
         <v>91</v>
       </c>
       <c r="B42" s="2"/>
@@ -5735,7 +5742,7 @@
       </c>
     </row>
     <row r="43" spans="1:36">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B43" s="2"/>
@@ -5843,7 +5850,7 @@
       </c>
     </row>
     <row r="44" spans="1:36">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="6" t="s">
         <v>217</v>
       </c>
       <c r="B44" s="2"/>
@@ -5951,7 +5958,7 @@
       </c>
     </row>
     <row r="45" spans="1:36">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="2"/>
@@ -6059,7 +6066,7 @@
       </c>
     </row>
     <row r="46" spans="1:36">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B46" s="2"/>
@@ -6167,7 +6174,7 @@
       </c>
     </row>
     <row r="47" spans="1:36">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="6" t="s">
         <v>133</v>
       </c>
       <c r="B47" s="2">
@@ -6277,7 +6284,7 @@
       </c>
     </row>
     <row r="48" spans="1:36">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="6" t="s">
         <v>162</v>
       </c>
       <c r="B48" s="2"/>
@@ -6385,7 +6392,7 @@
       </c>
     </row>
     <row r="49" spans="1:36">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="6" t="s">
         <v>106</v>
       </c>
       <c r="B49" s="2"/>
@@ -6493,7 +6500,7 @@
       </c>
     </row>
     <row r="50" spans="1:36">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="6" t="s">
         <v>175</v>
       </c>
       <c r="B50" s="2"/>
@@ -6601,7 +6608,7 @@
       </c>
     </row>
     <row r="51" spans="1:36">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="6" t="s">
         <v>200</v>
       </c>
       <c r="B51" s="2"/>
@@ -6709,7 +6716,7 @@
       </c>
     </row>
     <row r="52" spans="1:36">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="2"/>
@@ -6817,7 +6824,7 @@
       </c>
     </row>
     <row r="53" spans="1:36">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="6" t="s">
         <v>86</v>
       </c>
       <c r="B53" s="2"/>
@@ -6925,7 +6932,7 @@
       </c>
     </row>
     <row r="54" spans="1:36">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="6" t="s">
         <v>92</v>
       </c>
       <c r="B54" s="2"/>
@@ -7033,7 +7040,7 @@
       </c>
     </row>
     <row r="55" spans="1:36">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="6" t="s">
         <v>196</v>
       </c>
       <c r="B55" s="2"/>
@@ -7141,7 +7148,7 @@
       </c>
     </row>
     <row r="56" spans="1:36">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="6" t="s">
         <v>156</v>
       </c>
       <c r="B56" s="2"/>
@@ -7249,7 +7256,7 @@
       </c>
     </row>
     <row r="57" spans="1:36">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="6" t="s">
         <v>230</v>
       </c>
       <c r="B57" s="2"/>
@@ -7357,7 +7364,7 @@
       </c>
     </row>
     <row r="58" spans="1:36">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="6" t="s">
         <v>164</v>
       </c>
       <c r="B58" s="2"/>
@@ -7465,7 +7472,7 @@
       </c>
     </row>
     <row r="59" spans="1:36">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="6" t="s">
         <v>121</v>
       </c>
       <c r="B59" s="2"/>
@@ -7573,7 +7580,7 @@
       </c>
     </row>
     <row r="60" spans="1:36">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="6" t="s">
         <v>197</v>
       </c>
       <c r="B60" s="2"/>
@@ -7681,7 +7688,7 @@
       </c>
     </row>
     <row r="61" spans="1:36">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="6" t="s">
         <v>90</v>
       </c>
       <c r="B61" s="2"/>
@@ -7789,7 +7796,7 @@
       </c>
     </row>
     <row r="62" spans="1:36">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B62" s="2"/>
@@ -7897,7 +7904,7 @@
       </c>
     </row>
     <row r="63" spans="1:36">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B63" s="2"/>
@@ -8005,7 +8012,7 @@
       </c>
     </row>
     <row r="64" spans="1:36">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B64" s="2">
@@ -8115,7 +8122,7 @@
       </c>
     </row>
     <row r="65" spans="1:36">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="6" t="s">
         <v>74</v>
       </c>
       <c r="B65" s="2"/>
@@ -8223,7 +8230,7 @@
       </c>
     </row>
     <row r="66" spans="1:36">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B66" s="2"/>
@@ -8331,7 +8338,7 @@
       </c>
     </row>
     <row r="67" spans="1:36">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B67" s="2"/>
@@ -8439,7 +8446,7 @@
       </c>
     </row>
     <row r="68" spans="1:36">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B68" s="2"/>
@@ -8547,7 +8554,7 @@
       </c>
     </row>
     <row r="69" spans="1:36">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="6" t="s">
         <v>211</v>
       </c>
       <c r="B69" s="2"/>
@@ -8655,7 +8662,7 @@
       </c>
     </row>
     <row r="70" spans="1:36">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B70" s="2"/>
@@ -8763,7 +8770,7 @@
       </c>
     </row>
     <row r="71" spans="1:36">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="6" t="s">
         <v>96</v>
       </c>
       <c r="B71" s="2"/>
@@ -8871,7 +8878,7 @@
       </c>
     </row>
     <row r="72" spans="1:36">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="6" t="s">
         <v>146</v>
       </c>
       <c r="B72" s="2"/>
@@ -8979,7 +8986,7 @@
       </c>
     </row>
     <row r="73" spans="1:36">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="6" t="s">
         <v>149</v>
       </c>
       <c r="B73" s="2"/>
@@ -9087,7 +9094,7 @@
       </c>
     </row>
     <row r="74" spans="1:36">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="6" t="s">
         <v>206</v>
       </c>
       <c r="B74" s="2"/>
@@ -9195,7 +9202,7 @@
       </c>
     </row>
     <row r="75" spans="1:36">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="6" t="s">
         <v>188</v>
       </c>
       <c r="B75" s="2"/>
@@ -9303,7 +9310,7 @@
       </c>
     </row>
     <row r="76" spans="1:36">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="6" t="s">
         <v>155</v>
       </c>
       <c r="B76" s="2"/>
@@ -9411,7 +9418,7 @@
       </c>
     </row>
     <row r="77" spans="1:36">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="6" t="s">
         <v>135</v>
       </c>
       <c r="B77" s="2"/>
@@ -9519,7 +9526,7 @@
       </c>
     </row>
     <row r="78" spans="1:36">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="6" t="s">
         <v>169</v>
       </c>
       <c r="B78" s="2"/>
@@ -9627,7 +9634,7 @@
       </c>
     </row>
     <row r="79" spans="1:36">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="6" t="s">
         <v>161</v>
       </c>
       <c r="B79" s="2"/>
@@ -9735,7 +9742,7 @@
       </c>
     </row>
     <row r="80" spans="1:36">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="6" t="s">
         <v>201</v>
       </c>
       <c r="B80" s="2"/>
@@ -9843,7 +9850,7 @@
       </c>
     </row>
     <row r="81" spans="1:36">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="6" t="s">
         <v>202</v>
       </c>
       <c r="B81" s="2"/>
@@ -9951,7 +9958,7 @@
       </c>
     </row>
     <row r="82" spans="1:36">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B82" s="2"/>
@@ -10059,7 +10066,7 @@
       </c>
     </row>
     <row r="83" spans="1:36">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B83" s="2"/>
@@ -10167,7 +10174,7 @@
       </c>
     </row>
     <row r="84" spans="1:36">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="6" t="s">
         <v>231</v>
       </c>
       <c r="B84" s="2"/>
@@ -10275,7 +10282,7 @@
       </c>
     </row>
     <row r="85" spans="1:36">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="6" t="s">
         <v>122</v>
       </c>
       <c r="B85" s="2"/>
@@ -10383,7 +10390,7 @@
       </c>
     </row>
     <row r="86" spans="1:36">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="6" t="s">
         <v>154</v>
       </c>
       <c r="B86" s="2"/>
@@ -10491,7 +10498,7 @@
       </c>
     </row>
     <row r="87" spans="1:36">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B87" s="2"/>
@@ -10599,7 +10606,7 @@
       </c>
     </row>
     <row r="88" spans="1:36">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B88" s="2"/>
@@ -10707,7 +10714,7 @@
       </c>
     </row>
     <row r="89" spans="1:36">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="6" t="s">
         <v>208</v>
       </c>
       <c r="B89" s="2"/>
@@ -10815,7 +10822,7 @@
       </c>
     </row>
     <row r="90" spans="1:36">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="6" t="s">
         <v>187</v>
       </c>
       <c r="B90" s="2"/>
@@ -10923,7 +10930,7 @@
       </c>
     </row>
     <row r="91" spans="1:36">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B91" s="2"/>
@@ -11031,7 +11038,7 @@
       </c>
     </row>
     <row r="92" spans="1:36">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B92" s="2"/>
@@ -11139,7 +11146,7 @@
       </c>
     </row>
     <row r="93" spans="1:36">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="6" t="s">
         <v>118</v>
       </c>
       <c r="B93" s="2"/>
@@ -11247,7 +11254,7 @@
       </c>
     </row>
     <row r="94" spans="1:36">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B94" s="2"/>
@@ -11355,7 +11362,7 @@
       </c>
     </row>
     <row r="95" spans="1:36">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="6" t="s">
         <v>185</v>
       </c>
       <c r="B95" s="2"/>
@@ -11463,7 +11470,7 @@
       </c>
     </row>
     <row r="96" spans="1:36">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="6" t="s">
         <v>137</v>
       </c>
       <c r="B96" s="2"/>
@@ -11571,7 +11578,7 @@
       </c>
     </row>
     <row r="97" spans="1:36">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B97" s="2"/>
@@ -11679,7 +11686,7 @@
       </c>
     </row>
     <row r="98" spans="1:36">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="6" t="s">
         <v>212</v>
       </c>
       <c r="B98" s="2"/>
@@ -11787,7 +11794,7 @@
       </c>
     </row>
     <row r="99" spans="1:36">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="6" t="s">
         <v>126</v>
       </c>
       <c r="B99" s="2"/>
@@ -11895,7 +11902,7 @@
       </c>
     </row>
     <row r="100" spans="1:36">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B100" s="2"/>
@@ -12003,7 +12010,7 @@
       </c>
     </row>
     <row r="101" spans="1:36">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B101" s="2"/>
@@ -12111,7 +12118,7 @@
       </c>
     </row>
     <row r="102" spans="1:36">
-      <c r="A102" s="2" t="s">
+      <c r="A102" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B102" s="2"/>
@@ -12219,7 +12226,7 @@
       </c>
     </row>
     <row r="103" spans="1:36">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="6" t="s">
         <v>222</v>
       </c>
       <c r="B103" s="2"/>
@@ -12327,7 +12334,7 @@
       </c>
     </row>
     <row r="104" spans="1:36">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="6" t="s">
         <v>125</v>
       </c>
       <c r="B104" s="2"/>
@@ -12435,7 +12442,7 @@
       </c>
     </row>
     <row r="105" spans="1:36">
-      <c r="A105" s="2" t="s">
+      <c r="A105" s="6" t="s">
         <v>136</v>
       </c>
       <c r="B105" s="2"/>
@@ -12543,7 +12550,7 @@
       </c>
     </row>
     <row r="106" spans="1:36">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B106" s="2"/>
@@ -12651,7 +12658,7 @@
       </c>
     </row>
     <row r="107" spans="1:36">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="6" t="s">
         <v>179</v>
       </c>
       <c r="B107" s="2"/>
@@ -12759,7 +12766,7 @@
       </c>
     </row>
     <row r="108" spans="1:36">
-      <c r="A108" s="2" t="s">
+      <c r="A108" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B108" s="2"/>
@@ -12867,7 +12874,7 @@
       </c>
     </row>
     <row r="109" spans="1:36">
-      <c r="A109" s="2" t="s">
+      <c r="A109" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B109" s="2"/>
@@ -12975,7 +12982,7 @@
       </c>
     </row>
     <row r="110" spans="1:36">
-      <c r="A110" s="2" t="s">
+      <c r="A110" s="6" t="s">
         <v>172</v>
       </c>
       <c r="B110" s="2"/>
@@ -13083,7 +13090,7 @@
       </c>
     </row>
     <row r="111" spans="1:36">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B111" s="2"/>
@@ -13191,7 +13198,7 @@
       </c>
     </row>
     <row r="112" spans="1:36">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B112" s="2"/>
@@ -13299,7 +13306,7 @@
       </c>
     </row>
     <row r="113" spans="1:36">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B113" s="2"/>
@@ -13407,7 +13414,7 @@
       </c>
     </row>
     <row r="114" spans="1:36">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B114" s="2"/>
@@ -13515,7 +13522,7 @@
       </c>
     </row>
     <row r="115" spans="1:36">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="6" t="s">
         <v>180</v>
       </c>
       <c r="B115" s="2"/>
@@ -13623,7 +13630,7 @@
       </c>
     </row>
     <row r="116" spans="1:36">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B116" s="2"/>
@@ -13731,7 +13738,7 @@
       </c>
     </row>
     <row r="117" spans="1:36">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B117" s="2"/>
@@ -13839,7 +13846,7 @@
       </c>
     </row>
     <row r="118" spans="1:36">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B118" s="2"/>
@@ -13947,7 +13954,7 @@
       </c>
     </row>
     <row r="119" spans="1:36">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="6" t="s">
         <v>184</v>
       </c>
       <c r="B119" s="2"/>
@@ -14055,7 +14062,7 @@
       </c>
     </row>
     <row r="120" spans="1:36">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="6" t="s">
         <v>159</v>
       </c>
       <c r="B120" s="2"/>
@@ -14163,7 +14170,7 @@
       </c>
     </row>
     <row r="121" spans="1:36">
-      <c r="A121" s="2" t="s">
+      <c r="A121" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B121" s="2"/>
@@ -14271,7 +14278,7 @@
       </c>
     </row>
     <row r="122" spans="1:36">
-      <c r="A122" s="2" t="s">
+      <c r="A122" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B122" s="2"/>
@@ -14379,7 +14386,7 @@
       </c>
     </row>
     <row r="123" spans="1:36">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="6" t="s">
         <v>114</v>
       </c>
       <c r="B123" s="2"/>
@@ -14487,7 +14494,7 @@
       </c>
     </row>
     <row r="124" spans="1:36">
-      <c r="A124" s="2" t="s">
+      <c r="A124" s="6" t="s">
         <v>195</v>
       </c>
       <c r="B124" s="2"/>
@@ -14595,7 +14602,7 @@
       </c>
     </row>
     <row r="125" spans="1:36">
-      <c r="A125" s="2" t="s">
+      <c r="A125" s="6" t="s">
         <v>76</v>
       </c>
       <c r="B125" s="2"/>
@@ -14703,7 +14710,7 @@
       </c>
     </row>
     <row r="126" spans="1:36">
-      <c r="A126" s="2" t="s">
+      <c r="A126" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B126" s="2"/>
@@ -14811,7 +14818,7 @@
       </c>
     </row>
     <row r="127" spans="1:36">
-      <c r="A127" s="2" t="s">
+      <c r="A127" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B127" s="2"/>
@@ -14919,7 +14926,7 @@
       </c>
     </row>
     <row r="128" spans="1:36">
-      <c r="A128" s="2" t="s">
+      <c r="A128" s="6" t="s">
         <v>226</v>
       </c>
       <c r="B128" s="2"/>
@@ -15027,7 +15034,7 @@
       </c>
     </row>
     <row r="129" spans="1:36">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B129" s="2"/>
@@ -15135,7 +15142,7 @@
       </c>
     </row>
     <row r="130" spans="1:36">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B130" s="2"/>
@@ -15243,7 +15250,7 @@
       </c>
     </row>
     <row r="131" spans="1:36">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="6" t="s">
         <v>128</v>
       </c>
       <c r="B131" s="2"/>
@@ -15351,7 +15358,7 @@
       </c>
     </row>
     <row r="132" spans="1:36">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="6" t="s">
         <v>124</v>
       </c>
       <c r="B132" s="2"/>
@@ -15459,7 +15466,7 @@
       </c>
     </row>
     <row r="133" spans="1:36">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="6" t="s">
         <v>150</v>
       </c>
       <c r="B133" s="2"/>
@@ -15567,7 +15574,7 @@
       </c>
     </row>
     <row r="134" spans="1:36">
-      <c r="A134" s="2" t="s">
+      <c r="A134" s="6" t="s">
         <v>205</v>
       </c>
       <c r="B134" s="2"/>
@@ -15675,7 +15682,7 @@
       </c>
     </row>
     <row r="135" spans="1:36">
-      <c r="A135" s="2" t="s">
+      <c r="A135" s="6" t="s">
         <v>190</v>
       </c>
       <c r="B135" s="2"/>
@@ -15783,7 +15790,7 @@
       </c>
     </row>
     <row r="136" spans="1:36">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B136" s="2"/>
@@ -15891,7 +15898,7 @@
       </c>
     </row>
     <row r="137" spans="1:36">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="6" t="s">
         <v>116</v>
       </c>
       <c r="B137" s="2"/>
@@ -15999,7 +16006,7 @@
       </c>
     </row>
     <row r="138" spans="1:36">
-      <c r="A138" s="2" t="s">
+      <c r="A138" s="6" t="s">
         <v>232</v>
       </c>
       <c r="B138" s="2"/>
@@ -16107,7 +16114,7 @@
       </c>
     </row>
     <row r="139" spans="1:36">
-      <c r="A139" s="2" t="s">
+      <c r="A139" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B139" s="2"/>
@@ -16215,7 +16222,7 @@
       </c>
     </row>
     <row r="140" spans="1:36">
-      <c r="A140" s="2" t="s">
+      <c r="A140" s="6" t="s">
         <v>176</v>
       </c>
       <c r="B140" s="2"/>
@@ -16323,7 +16330,7 @@
       </c>
     </row>
     <row r="141" spans="1:36">
-      <c r="A141" s="2" t="s">
+      <c r="A141" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B141" s="2"/>
@@ -16431,7 +16438,7 @@
       </c>
     </row>
     <row r="142" spans="1:36">
-      <c r="A142" s="2" t="s">
+      <c r="A142" s="6" t="s">
         <v>204</v>
       </c>
       <c r="B142" s="2"/>
@@ -16539,7 +16546,7 @@
       </c>
     </row>
     <row r="143" spans="1:36">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B143" s="2"/>
@@ -16647,7 +16654,7 @@
       </c>
     </row>
     <row r="144" spans="1:36">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B144" s="2"/>
@@ -16755,7 +16762,7 @@
       </c>
     </row>
     <row r="145" spans="1:36">
-      <c r="A145" s="2" t="s">
+      <c r="A145" s="6" t="s">
         <v>129</v>
       </c>
       <c r="B145" s="2"/>
@@ -16863,7 +16870,7 @@
       </c>
     </row>
     <row r="146" spans="1:36">
-      <c r="A146" s="2" t="s">
+      <c r="A146" s="6" t="s">
         <v>130</v>
       </c>
       <c r="B146" s="2"/>
@@ -16971,7 +16978,7 @@
       </c>
     </row>
     <row r="147" spans="1:36">
-      <c r="A147" s="2" t="s">
+      <c r="A147" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B147" s="2"/>
@@ -17079,7 +17086,7 @@
       </c>
     </row>
     <row r="148" spans="1:36">
-      <c r="A148" s="2" t="s">
+      <c r="A148" s="6" t="s">
         <v>182</v>
       </c>
       <c r="B148" s="2"/>
@@ -17187,7 +17194,7 @@
       </c>
     </row>
     <row r="149" spans="1:36">
-      <c r="A149" s="2" t="s">
+      <c r="A149" s="6" t="s">
         <v>209</v>
       </c>
       <c r="B149" s="2"/>
@@ -17295,7 +17302,7 @@
       </c>
     </row>
     <row r="150" spans="1:36">
-      <c r="A150" s="2" t="s">
+      <c r="A150" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B150" s="2"/>
@@ -17403,7 +17410,7 @@
       </c>
     </row>
     <row r="151" spans="1:36">
-      <c r="A151" s="2" t="s">
+      <c r="A151" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B151" s="2"/>
@@ -17511,7 +17518,7 @@
       </c>
     </row>
     <row r="152" spans="1:36">
-      <c r="A152" s="2" t="s">
+      <c r="A152" s="6" t="s">
         <v>177</v>
       </c>
       <c r="B152" s="2"/>
@@ -17619,7 +17626,7 @@
       </c>
     </row>
     <row r="153" spans="1:36">
-      <c r="A153" s="2" t="s">
+      <c r="A153" s="6" t="s">
         <v>218</v>
       </c>
       <c r="B153" s="2"/>
@@ -17727,7 +17734,7 @@
       </c>
     </row>
     <row r="154" spans="1:36">
-      <c r="A154" s="2" t="s">
+      <c r="A154" s="6" t="s">
         <v>207</v>
       </c>
       <c r="B154" s="2"/>
@@ -17835,7 +17842,7 @@
       </c>
     </row>
     <row r="155" spans="1:36">
-      <c r="A155" s="2" t="s">
+      <c r="A155" s="6" t="s">
         <v>225</v>
       </c>
       <c r="B155" s="2"/>
@@ -17943,7 +17950,7 @@
       </c>
     </row>
     <row r="156" spans="1:36">
-      <c r="A156" s="2" t="s">
+      <c r="A156" s="6" t="s">
         <v>79</v>
       </c>
       <c r="B156" s="2"/>
@@ -18051,7 +18058,7 @@
       </c>
     </row>
     <row r="157" spans="1:36">
-      <c r="A157" s="2" t="s">
+      <c r="A157" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B157" s="2"/>
@@ -18159,7 +18166,7 @@
       </c>
     </row>
     <row r="158" spans="1:36">
-      <c r="A158" s="2" t="s">
+      <c r="A158" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B158" s="2"/>
@@ -18267,7 +18274,7 @@
       </c>
     </row>
     <row r="159" spans="1:36">
-      <c r="A159" s="2" t="s">
+      <c r="A159" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B159" s="2"/>
@@ -18375,7 +18382,7 @@
       </c>
     </row>
     <row r="160" spans="1:36">
-      <c r="A160" s="2" t="s">
+      <c r="A160" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B160" s="2"/>
@@ -18483,7 +18490,7 @@
       </c>
     </row>
     <row r="161" spans="1:36">
-      <c r="A161" s="2" t="s">
+      <c r="A161" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B161" s="2"/>
@@ -18591,7 +18598,7 @@
       </c>
     </row>
     <row r="162" spans="1:36">
-      <c r="A162" s="2" t="s">
+      <c r="A162" s="6" t="s">
         <v>127</v>
       </c>
       <c r="B162" s="2"/>
@@ -18699,7 +18706,7 @@
       </c>
     </row>
     <row r="163" spans="1:36">
-      <c r="A163" s="2" t="s">
+      <c r="A163" s="6" t="s">
         <v>131</v>
       </c>
       <c r="B163" s="2"/>
@@ -18807,7 +18814,7 @@
       </c>
     </row>
     <row r="164" spans="1:36">
-      <c r="A164" s="2" t="s">
+      <c r="A164" s="6" t="s">
         <v>138</v>
       </c>
       <c r="B164" s="2"/>
@@ -18915,7 +18922,7 @@
       </c>
     </row>
     <row r="165" spans="1:36">
-      <c r="A165" s="2" t="s">
+      <c r="A165" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B165" s="2"/>
@@ -19023,7 +19030,7 @@
       </c>
     </row>
     <row r="166" spans="1:36">
-      <c r="A166" s="2" t="s">
+      <c r="A166" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B166" s="2"/>
@@ -19131,7 +19138,7 @@
       </c>
     </row>
     <row r="167" spans="1:36">
-      <c r="A167" s="2" t="s">
+      <c r="A167" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B167" s="2"/>
@@ -19239,7 +19246,7 @@
       </c>
     </row>
     <row r="168" spans="1:36">
-      <c r="A168" s="2" t="s">
+      <c r="A168" s="6" t="s">
         <v>191</v>
       </c>
       <c r="B168" s="2"/>
@@ -19347,7 +19354,7 @@
       </c>
     </row>
     <row r="169" spans="1:36">
-      <c r="A169" s="2" t="s">
+      <c r="A169" s="6" t="s">
         <v>142</v>
       </c>
       <c r="B169" s="2"/>
@@ -19455,7 +19462,7 @@
       </c>
     </row>
     <row r="170" spans="1:36">
-      <c r="A170" s="2" t="s">
+      <c r="A170" s="6" t="s">
         <v>100</v>
       </c>
       <c r="B170" s="2"/>
@@ -19563,7 +19570,7 @@
       </c>
     </row>
     <row r="171" spans="1:36">
-      <c r="A171" s="2" t="s">
+      <c r="A171" s="6" t="s">
         <v>119</v>
       </c>
       <c r="B171" s="2"/>
@@ -19671,7 +19678,7 @@
       </c>
     </row>
     <row r="172" spans="1:36">
-      <c r="A172" s="2" t="s">
+      <c r="A172" s="6" t="s">
         <v>223</v>
       </c>
       <c r="B172" s="2"/>
@@ -19779,7 +19786,7 @@
       </c>
     </row>
     <row r="173" spans="1:36">
-      <c r="A173" s="2" t="s">
+      <c r="A173" s="6" t="s">
         <v>227</v>
       </c>
       <c r="B173" s="2"/>
@@ -19887,7 +19894,7 @@
       </c>
     </row>
     <row r="174" spans="1:36">
-      <c r="A174" s="2" t="s">
+      <c r="A174" s="6" t="s">
         <v>228</v>
       </c>
       <c r="B174" s="2"/>
@@ -19995,7 +20002,7 @@
       </c>
     </row>
     <row r="175" spans="1:36">
-      <c r="A175" s="2" t="s">
+      <c r="A175" s="6" t="s">
         <v>139</v>
       </c>
       <c r="B175" s="2"/>
@@ -20103,7 +20110,7 @@
       </c>
     </row>
     <row r="176" spans="1:36">
-      <c r="A176" s="2" t="s">
+      <c r="A176" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B176" s="2"/>
@@ -20211,7 +20218,7 @@
       </c>
     </row>
     <row r="177" spans="1:36">
-      <c r="A177" s="2" t="s">
+      <c r="A177" s="6" t="s">
         <v>203</v>
       </c>
       <c r="B177" s="2"/>
@@ -20319,7 +20326,7 @@
       </c>
     </row>
     <row r="178" spans="1:36">
-      <c r="A178" s="2" t="s">
+      <c r="A178" s="6" t="s">
         <v>134</v>
       </c>
       <c r="B178" s="2"/>
@@ -20427,7 +20434,7 @@
       </c>
     </row>
     <row r="179" spans="1:36">
-      <c r="A179" s="2" t="s">
+      <c r="A179" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B179" s="2"/>
@@ -20535,7 +20542,7 @@
       </c>
     </row>
     <row r="180" spans="1:36">
-      <c r="A180" s="2" t="s">
+      <c r="A180" s="6" t="s">
         <v>166</v>
       </c>
       <c r="B180" s="2"/>
@@ -20643,7 +20650,7 @@
       </c>
     </row>
     <row r="181" spans="1:36">
-      <c r="A181" s="2" t="s">
+      <c r="A181" s="6" t="s">
         <v>157</v>
       </c>
       <c r="B181" s="2"/>
@@ -20751,7 +20758,7 @@
       </c>
     </row>
     <row r="182" spans="1:36">
-      <c r="A182" s="2" t="s">
+      <c r="A182" s="6" t="s">
         <v>107</v>
       </c>
       <c r="B182" s="2"/>
@@ -20859,7 +20866,7 @@
       </c>
     </row>
     <row r="183" spans="1:36">
-      <c r="A183" s="2" t="s">
+      <c r="A183" s="6" t="s">
         <v>173</v>
       </c>
       <c r="B183" s="2"/>
@@ -20967,7 +20974,7 @@
       </c>
     </row>
     <row r="184" spans="1:36">
-      <c r="A184" s="2" t="s">
+      <c r="A184" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B184" s="2"/>
@@ -21075,7 +21082,7 @@
       </c>
     </row>
     <row r="185" spans="1:36">
-      <c r="A185" s="2" t="s">
+      <c r="A185" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B185" s="2"/>
@@ -21183,7 +21190,7 @@
       </c>
     </row>
     <row r="186" spans="1:36">
-      <c r="A186" s="2" t="s">
+      <c r="A186" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B186" s="2"/>
@@ -21291,7 +21298,7 @@
       </c>
     </row>
     <row r="187" spans="1:36">
-      <c r="A187" s="2" t="s">
+      <c r="A187" s="6" t="s">
         <v>168</v>
       </c>
       <c r="B187" s="2"/>
@@ -21399,7 +21406,7 @@
       </c>
     </row>
     <row r="188" spans="1:36">
-      <c r="A188" s="2" t="s">
+      <c r="A188" s="6" t="s">
         <v>181</v>
       </c>
       <c r="B188" s="2"/>
@@ -21507,7 +21514,7 @@
       </c>
     </row>
     <row r="189" spans="1:36">
-      <c r="A189" s="2" t="s">
+      <c r="A189" s="6" t="s">
         <v>140</v>
       </c>
       <c r="B189" s="2"/>
@@ -21615,7 +21622,7 @@
       </c>
     </row>
     <row r="190" spans="1:36">
-      <c r="A190" s="2" t="s">
+      <c r="A190" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B190" s="2"/>
@@ -21723,7 +21730,7 @@
       </c>
     </row>
     <row r="191" spans="1:36">
-      <c r="A191" s="2" t="s">
+      <c r="A191" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B191" s="2"/>
@@ -21831,7 +21838,7 @@
       </c>
     </row>
     <row r="192" spans="1:36">
-      <c r="A192" s="2" t="s">
+      <c r="A192" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B192" s="2"/>
@@ -21939,7 +21946,7 @@
       </c>
     </row>
     <row r="193" spans="1:36">
-      <c r="A193" s="2" t="s">
+      <c r="A193" s="6" t="s">
         <v>178</v>
       </c>
       <c r="B193" s="2"/>
@@ -22047,7 +22054,7 @@
       </c>
     </row>
     <row r="194" spans="1:36">
-      <c r="A194" s="2" t="s">
+      <c r="A194" s="6" t="s">
         <v>186</v>
       </c>
       <c r="B194" s="2"/>
@@ -22155,7 +22162,7 @@
       </c>
     </row>
     <row r="195" spans="1:36">
-      <c r="A195" s="2" t="s">
+      <c r="A195" s="6" t="s">
         <v>167</v>
       </c>
       <c r="B195" s="2"/>
@@ -22263,7 +22270,7 @@
       </c>
     </row>
     <row r="196" spans="1:36">
-      <c r="A196" s="2" t="s">
+      <c r="A196" s="6" t="s">
         <v>151</v>
       </c>
       <c r="B196" s="2"/>
@@ -22371,7 +22378,7 @@
       </c>
     </row>
     <row r="197" spans="1:36">
-      <c r="A197" s="2" t="s">
+      <c r="A197" s="6" t="s">
         <v>141</v>
       </c>
       <c r="B197" s="2"/>
@@ -22479,7 +22486,7 @@
       </c>
     </row>
     <row r="198" spans="1:36">
-      <c r="A198" s="2" t="s">
+      <c r="A198" s="6" t="s">
         <v>171</v>
       </c>
       <c r="B198" s="2"/>
@@ -22587,7 +22594,7 @@
       </c>
     </row>
     <row r="199" spans="1:36">
-      <c r="A199" s="2" t="s">
+      <c r="A199" s="6" t="s">
         <v>174</v>
       </c>
       <c r="B199" s="2"/>
@@ -22695,7 +22702,7 @@
       </c>
     </row>
     <row r="200" spans="1:36">
-      <c r="A200" s="2" t="s">
+      <c r="A200" s="6" t="s">
         <v>229</v>
       </c>
       <c r="B200" s="2"/>
@@ -22803,7 +22810,7 @@
       </c>
     </row>
     <row r="201" spans="1:36">
-      <c r="A201" s="2" t="s">
+      <c r="A201" s="6" t="s">
         <v>214</v>
       </c>
       <c r="B201" s="2"/>
@@ -22911,7 +22918,7 @@
       </c>
     </row>
     <row r="202" spans="1:36">
-      <c r="A202" s="2" t="s">
+      <c r="A202" s="6" t="s">
         <v>224</v>
       </c>
       <c r="B202" s="2"/>

</xml_diff>